<commit_message>
finish check date report
</commit_message>
<xml_diff>
--- a/src/main/resources/download/BC_RESULT_TRANSMIT.xlsx
+++ b/src/main/resources/download/BC_RESULT_TRANSMIT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaWeb\KMS\kms\src\main\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DEV/Projects/KMS/kms/src/main/resources/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A62C76-860C-D541-9D2C-341CCDCDCD39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="465" windowWidth="23265" windowHeight="12585"/>
+    <workbookView xWindow="2180" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -338,13 +339,13 @@
     <t>${bean.confirmDate}</t>
   </si>
   <si>
-    <t>${bean.timeRead/60000}</t>
+    <t>${bean.timeRead/60000.0}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
     <numFmt numFmtId="165" formatCode="[$-409]dddd\,\ mmmm\ d\,\ yyyy"/>
@@ -546,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -601,12 +602,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -628,6 +623,48 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -637,55 +674,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -936,6 +940,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -971,6 +992,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1146,61 +1184,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="32.1640625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="21" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" style="21" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" customWidth="1"/>
+    <col min="2" max="2" width="19.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" customWidth="1"/>
+    <col min="4" max="4" width="22.3984375" customWidth="1"/>
+    <col min="5" max="5" width="18.3984375" customWidth="1"/>
+    <col min="6" max="6" width="24.59765625" customWidth="1"/>
+    <col min="7" max="7" width="32.19921875" style="19" customWidth="1"/>
+    <col min="8" max="8" width="20.59765625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="20.796875" style="19" customWidth="1"/>
+    <col min="10" max="10" width="23.3984375" style="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:6" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="1:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+    </row>
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.15">
+      <c r="A4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1208,37 +1246,37 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="64.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
+    <row r="6" spans="1:6" ht="64.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
-    </row>
-    <row r="8" spans="1:6" ht="43.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38"/>
+    </row>
+    <row r="8" spans="1:6" ht="43.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+    </row>
+    <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="14" t="s">
         <v>18</v>
       </c>
@@ -1246,7 +1284,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1256,17 +1294,17 @@
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="12" t="s">
         <v>21</v>
       </c>
@@ -1274,7 +1312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1284,31 +1322,31 @@
       <c r="E12" s="10"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="36"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="8"/>
       <c r="F13" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="61.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+    <row r="14" spans="1:6" ht="61.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1316,39 +1354,39 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="86.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+    <row r="16" spans="1:6" ht="86.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-    </row>
-    <row r="22" spans="1:10" ht="34.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="30" t="s">
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+    </row>
+    <row r="22" spans="1:10" ht="34.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="24"/>
-    </row>
-    <row r="24" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G23" s="22"/>
+    </row>
+    <row r="24" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A24" s="15" t="s">
         <v>3</v>
       </c>
@@ -1367,20 +1405,20 @@
       <c r="F24" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="22" t="s">
+      <c r="I24" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="J24" s="18" t="s">
+      <c r="J24" s="45" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
@@ -1389,12 +1427,12 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="19"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G25" s="24"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="46"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>12</v>
       </c>
@@ -1410,23 +1448,23 @@
       <c r="E26" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="45" t="s">
+      <c r="F26" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="44" t="s">
+      <c r="G26" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="H26" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="I26" s="20" t="s">
+      <c r="I26" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="J26" s="46" t="s">
+      <c r="J26" s="47" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
         <v>14</v>
       </c>
@@ -1435,13 +1473,18 @@
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="19"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="A1:C1"/>
@@ -1450,11 +1493,6 @@
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>